<commit_message>
Added the send_mail function that attaches the excel and sends email using outlook to the list of suppliers.
</commit_message>
<xml_diff>
--- a/RFQ_Excel/5995/hardware.xlsx
+++ b/RFQ_Excel/5995/hardware.xlsx
@@ -675,6 +675,9 @@
           <t>INSERT-MS-21209-11-15</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -687,6 +690,9 @@
           <t>NUTPLATE-MS21061-3</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -699,6 +705,9 @@
           <t>RIV - MS20426AD3-3</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>05-10411
@@ -718,6 +727,9 @@
           <t>NUTPLATE - MS21075L3N</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -729,6 +741,9 @@
         <is>
           <t>Testing Tool - 2</t>
         </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>